<commit_message>
Update tugas 1, penambahan argumen, adaptive excel import (enable and disable), penambahan struct (dictionary), penambahan last id agar dapat adaptable dengan lintas function, penbamahan tambahAnggota(), untuk menambahkan anggota dengan (tambahAnggota(string nama, alamat, pekerjaan, alasan)), penambahan excelToKelas() dengan menggunakan excelise, lalu open file excel, get row, row tersebut dimasukkan ke variable struct, ditambahkan melalui perulangan for, lalu akhirnya ditambahkan melalui append.
</commit_message>
<xml_diff>
--- a/Tugas_1/Kelas.xlsx
+++ b/Tugas_1/Kelas.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Program\GoWorkspace\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Program\GoWorkspace\Kominfo_Golang\Tugas_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B1A879-E728-4C69-885D-92283507B1BB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{45BAD90F-CADB-4303-9F96-9FFA98462913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="109">
   <si>
     <r>
       <rPr>
@@ -1075,6 +1075,12 @@
   </si>
   <si>
     <t>Fresh Graduate Akademi Kominfo</t>
+  </si>
+  <si>
+    <t>Alasan</t>
+  </si>
+  <si>
+    <t>Kesempatan belajar golang</t>
   </si>
 </sst>
 </file>
@@ -1156,7 +1162,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1174,6 +1180,12 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1479,10 +1491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E201"/>
+  <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A89" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="D44" sqref="D44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1490,11 +1502,11 @@
     <col min="1" max="1" width="6" customWidth="1"/>
     <col min="2" max="2" width="22" customWidth="1"/>
     <col min="3" max="4" width="41.33203125" customWidth="1"/>
-    <col min="5" max="5" width="42" customWidth="1"/>
-    <col min="6" max="6" width="2.6640625" customWidth="1"/>
+    <col min="5" max="6" width="42" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1510,8 +1522,11 @@
       <c r="E1" s="5" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="6" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>151</v>
       </c>
@@ -1527,8 +1542,11 @@
       <c r="E2" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F2" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>152</v>
       </c>
@@ -1544,8 +1562,11 @@
       <c r="E3" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F3" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>153</v>
       </c>
@@ -1561,8 +1582,11 @@
       <c r="E4" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F4" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>154</v>
       </c>
@@ -1578,8 +1602,11 @@
       <c r="E5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F5" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>155</v>
       </c>
@@ -1595,8 +1622,11 @@
       <c r="E6" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F6" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>156</v>
       </c>
@@ -1612,8 +1642,11 @@
       <c r="E7" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F7" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>157</v>
       </c>
@@ -1629,8 +1662,11 @@
       <c r="E8" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F8" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>158</v>
       </c>
@@ -1646,8 +1682,11 @@
       <c r="E9" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>159</v>
       </c>
@@ -1663,8 +1702,11 @@
       <c r="E10" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F10" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>160</v>
       </c>
@@ -1680,8 +1722,11 @@
       <c r="E11" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F11" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>161</v>
       </c>
@@ -1697,8 +1742,11 @@
       <c r="E12" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F12" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>162</v>
       </c>
@@ -1714,8 +1762,11 @@
       <c r="E13" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F13" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>163</v>
       </c>
@@ -1731,8 +1782,11 @@
       <c r="E14" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F14" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>164</v>
       </c>
@@ -1748,8 +1802,11 @@
       <c r="E15" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F15" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>165</v>
       </c>
@@ -1765,8 +1822,11 @@
       <c r="E16" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F16" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>166</v>
       </c>
@@ -1782,8 +1842,11 @@
       <c r="E17" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>167</v>
       </c>
@@ -1799,8 +1862,11 @@
       <c r="E18" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F18" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>168</v>
       </c>
@@ -1816,8 +1882,11 @@
       <c r="E19" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F19" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>169</v>
       </c>
@@ -1833,8 +1902,11 @@
       <c r="E20" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F20" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>170</v>
       </c>
@@ -1850,8 +1922,11 @@
       <c r="E21" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="22" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F21" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>171</v>
       </c>
@@ -1867,8 +1942,11 @@
       <c r="E22" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F22" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>172</v>
       </c>
@@ -1884,8 +1962,11 @@
       <c r="E23" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F23" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>173</v>
       </c>
@@ -1901,8 +1982,11 @@
       <c r="E24" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F24" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>174</v>
       </c>
@@ -1918,8 +2002,11 @@
       <c r="E25" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
         <v>175</v>
       </c>
@@ -1935,8 +2022,11 @@
       <c r="E26" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F26" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
         <v>176</v>
       </c>
@@ -1952,8 +2042,11 @@
       <c r="E27" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F27" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
         <v>177</v>
       </c>
@@ -1969,8 +2062,11 @@
       <c r="E28" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F28" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
         <v>178</v>
       </c>
@@ -1986,8 +2082,11 @@
       <c r="E29" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F29" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
         <v>179</v>
       </c>
@@ -2003,8 +2102,11 @@
       <c r="E30" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F30" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>180</v>
       </c>
@@ -2020,8 +2122,11 @@
       <c r="E31" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F31" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>181</v>
       </c>
@@ -2037,8 +2142,11 @@
       <c r="E32" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F32" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="3">
         <v>182</v>
       </c>
@@ -2054,8 +2162,11 @@
       <c r="E33" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F33" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="3">
         <v>183</v>
       </c>
@@ -2071,8 +2182,11 @@
       <c r="E34" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="35" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F34" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="3">
         <v>184</v>
       </c>
@@ -2088,8 +2202,11 @@
       <c r="E35" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F35" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="3">
         <v>185</v>
       </c>
@@ -2105,8 +2222,11 @@
       <c r="E36" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="37" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F36" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="3">
         <v>186</v>
       </c>
@@ -2122,8 +2242,11 @@
       <c r="E37" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F37" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="3">
         <v>187</v>
       </c>
@@ -2139,8 +2262,11 @@
       <c r="E38" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="39" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F38" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="3">
         <v>188</v>
       </c>
@@ -2156,8 +2282,11 @@
       <c r="E39" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F39" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="3">
         <v>189</v>
       </c>
@@ -2173,8 +2302,11 @@
       <c r="E40" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F40" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3">
         <v>190</v>
       </c>
@@ -2190,8 +2322,11 @@
       <c r="E41" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="42" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F41" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="3">
         <v>191</v>
       </c>
@@ -2207,8 +2342,11 @@
       <c r="E42" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="43" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F42" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>192</v>
       </c>
@@ -2224,8 +2362,11 @@
       <c r="E43" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F43" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>193</v>
       </c>
@@ -2241,8 +2382,11 @@
       <c r="E44" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F44" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="3">
         <v>194</v>
       </c>
@@ -2258,8 +2402,11 @@
       <c r="E45" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F45" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="3">
         <v>195</v>
       </c>
@@ -2275,8 +2422,11 @@
       <c r="E46" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F46" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="3">
         <v>196</v>
       </c>
@@ -2292,8 +2442,11 @@
       <c r="E47" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="48" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F47" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="3">
         <v>197</v>
       </c>
@@ -2309,8 +2462,11 @@
       <c r="E48" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F48" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="3">
         <v>198</v>
       </c>
@@ -2326,8 +2482,11 @@
       <c r="E49" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F49" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="3">
         <v>199</v>
       </c>
@@ -2343,8 +2502,11 @@
       <c r="E50" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="F50" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="3">
         <v>200</v>
       </c>
@@ -2360,20 +2522,23 @@
       <c r="E51" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="52" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="53" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="54" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="55" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="56" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="57" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="58" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="59" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="60" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="61" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="62" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="63" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="64" spans="1:5" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+      <c r="F51" s="7" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="53" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="54" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="55" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="56" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="57" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="58" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="59" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="60" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="61" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="62" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="63" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="64" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="65" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="66" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>
     <row r="67" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
1. Menambahkan random function. 2. Menambahkan data agar spreadsheet tidak monoton.
</commit_message>
<xml_diff>
--- a/Tugas_1/Kelas.xlsx
+++ b/Tugas_1/Kelas.xlsx
@@ -8,265 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Program\GoWorkspace\Kominfo_Golang\Tugas_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{45BAD90F-CADB-4303-9F96-9FFA98462913}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F033E9D-6DD4-47D6-B7A7-E27E0D64FB1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Table 1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="109">
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>No</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nomor Registrasi</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="9"/>
-        <color rgb="FFFFFFFF"/>
-        <rFont val="Tahoma"/>
-        <family val="2"/>
-      </rPr>
-      <t>Nama</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Scalable Web Service with Golang (Batch1)</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-46</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>ADITTIYA ASRIL</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-460</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>DERI FAUZI</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-464</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>FAIZAL AMRI</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-468</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>ALIF PUTRA DEWANTARA</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-473</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>MUHAMMAD AGUNG DWI PRASETIYO</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-474</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>Ilham Arifin</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-476</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>M. HALVI RAHMAN</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-48</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>KHAERUL LATIF</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-482</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>MUHAMMAD SEMAN</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>1957356840-486</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9"/>
-        <rFont val="Calibri"/>
-        <family val="1"/>
-      </rPr>
-      <t>IRFAN ZUHDI ABDILLAH</t>
-    </r>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="136">
   <si>
     <r>
       <rPr>
@@ -1074,13 +841,166 @@
     <t>Pekerjaan</t>
   </si>
   <si>
-    <t>Fresh Graduate Akademi Kominfo</t>
-  </si>
-  <si>
     <t>Alasan</t>
   </si>
   <si>
-    <t>Kesempatan belajar golang</t>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Nomor Registrasi</t>
+  </si>
+  <si>
+    <t>Nama</t>
+  </si>
+  <si>
+    <t>1957356840-46</t>
+  </si>
+  <si>
+    <t>ADITTIYA ASRIL</t>
+  </si>
+  <si>
+    <t>Jl. Kebon Jeruk No. 123</t>
+  </si>
+  <si>
+    <t>Software Engineer</t>
+  </si>
+  <si>
+    <t>Menyukai tantangan baru</t>
+  </si>
+  <si>
+    <t>1957356840-460</t>
+  </si>
+  <si>
+    <t>DERI FAUZI</t>
+  </si>
+  <si>
+    <t>Jl. Merdeka No. 45</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
+  </si>
+  <si>
+    <t>Ingin mengembangkan skill programming</t>
+  </si>
+  <si>
+    <t>1957356840-464</t>
+  </si>
+  <si>
+    <t>FAIZAL AMRI</t>
+  </si>
+  <si>
+    <t>Jl. Cihampelas No. 67</t>
+  </si>
+  <si>
+    <t>UI/UX Designer</t>
+  </si>
+  <si>
+    <t>Minat pada desain grafis</t>
+  </si>
+  <si>
+    <t>1957356840-468</t>
+  </si>
+  <si>
+    <t>ALIF PUTRA DEWANTARA</t>
+  </si>
+  <si>
+    <t>Jl. Pahlawan No. 89</t>
+  </si>
+  <si>
+    <t>Network Engineer</t>
+  </si>
+  <si>
+    <t>Passionate tentang jaringan komputer</t>
+  </si>
+  <si>
+    <t>1957356840-473</t>
+  </si>
+  <si>
+    <t>MUHAMMAD AGUNG DWI PRASETIYO</t>
+  </si>
+  <si>
+    <t>Jl. Ahmad Yani No. 12</t>
+  </si>
+  <si>
+    <t>System Administrator</t>
+  </si>
+  <si>
+    <t>Pengalaman dalam administrasi sistem</t>
+  </si>
+  <si>
+    <t>1957356840-474</t>
+  </si>
+  <si>
+    <t>Ilham Arifin</t>
+  </si>
+  <si>
+    <t>Jl. Sukajadi No. 34</t>
+  </si>
+  <si>
+    <t>Software Developer</t>
+  </si>
+  <si>
+    <t>Minat pada pengembangan aplikasi</t>
+  </si>
+  <si>
+    <t>1957356840-476</t>
+  </si>
+  <si>
+    <t>M. HALVI RAHMAN</t>
+  </si>
+  <si>
+    <t>Jl. Riau No. 56</t>
+  </si>
+  <si>
+    <t>IT Consultant</t>
+  </si>
+  <si>
+    <t>Memiliki keahlian konsultasi IT</t>
+  </si>
+  <si>
+    <t>1957356840-48</t>
+  </si>
+  <si>
+    <t>KHAERUL LATIF</t>
+  </si>
+  <si>
+    <t>Jl. Dago No. 78</t>
+  </si>
+  <si>
+    <t>Cloud Engineer</t>
+  </si>
+  <si>
+    <t>Berpengalaman dalam pengelolaan cloud</t>
+  </si>
+  <si>
+    <t>1957356840-482</t>
+  </si>
+  <si>
+    <t>MUHAMMAD SEMAN</t>
+  </si>
+  <si>
+    <t>Jl. Setiabudi No. 90</t>
+  </si>
+  <si>
+    <t>DevOps Engineer</t>
+  </si>
+  <si>
+    <t>Memiliki keterampilan DevOps</t>
+  </si>
+  <si>
+    <t>1957356840-486</t>
+  </si>
+  <si>
+    <t>IRFAN ZUHDI ABDILLAH</t>
+  </si>
+  <si>
+    <t>Jl. Cijerah No. 23</t>
+  </si>
+  <si>
+    <t>Cyber Security Analyst</t>
+  </si>
+  <si>
+    <t>Minat pada keamanan cyber</t>
   </si>
 </sst>
 </file>
@@ -1181,10 +1101,10 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1493,8 +1413,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="D44" sqref="D44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1508,22 +1428,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>83</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>1</v>
+        <v>84</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>85</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>104</v>
+        <v>80</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>105</v>
+        <v>81</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>107</v>
+        <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1531,199 +1451,208 @@
         <v>151</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>4</v>
+        <v>86</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>87</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
+        <f>A2+1</f>
         <v>152</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>6</v>
+        <v>91</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>7</v>
+        <v>92</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="F3" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>153</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>8</v>
+        <v>96</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>9</v>
+        <v>97</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F4" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
+        <f t="shared" si="0"/>
         <v>154</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>101</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>11</v>
+        <v>102</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="F5" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
+        <f t="shared" si="0"/>
         <v>155</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>12</v>
+        <v>106</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>13</v>
+        <v>107</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="F6" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
+        <f t="shared" si="0"/>
         <v>156</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>15</v>
+        <v>112</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="F7" s="7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="8" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
+        <f t="shared" si="0"/>
         <v>157</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
+        <v>116</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>17</v>
+        <v>117</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="F8" s="7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
+        <f t="shared" si="0"/>
         <v>158</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>18</v>
+        <v>121</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>19</v>
+        <v>122</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="10" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
+        <f t="shared" si="0"/>
         <v>159</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>20</v>
+        <v>126</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>21</v>
+        <v>127</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="11" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
+        <f t="shared" si="0"/>
         <v>160</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>22</v>
+        <v>131</v>
       </c>
       <c r="C11" s="4" t="s">
-        <v>23</v>
+        <v>132</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="E11" s="4" t="s">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="F11" s="7" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1731,19 +1660,19 @@
         <v>161</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>25</v>
+        <v>1</v>
       </c>
       <c r="D12" s="4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E12" s="4" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="F12" s="7" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1751,19 +1680,19 @@
         <v>162</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>26</v>
+        <v>2</v>
       </c>
       <c r="C13" s="4" t="s">
-        <v>27</v>
+        <v>3</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E13" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="14" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1771,19 +1700,19 @@
         <v>163</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>28</v>
+        <v>4</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>29</v>
+        <v>5</v>
       </c>
       <c r="D14" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E14" s="4" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F14" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1791,19 +1720,19 @@
         <v>164</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>31</v>
+        <v>7</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E15" s="4" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="F15" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1811,19 +1740,19 @@
         <v>165</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
       <c r="C16" s="4" t="s">
-        <v>33</v>
+        <v>9</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E16" s="4" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="F16" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1831,19 +1760,19 @@
         <v>166</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C17" s="4" t="s">
-        <v>35</v>
+        <v>11</v>
       </c>
       <c r="D17" s="4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E17" s="4" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="18" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1851,19 +1780,19 @@
         <v>167</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>36</v>
+        <v>12</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>37</v>
+        <v>13</v>
       </c>
       <c r="D18" s="4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E18" s="4" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1871,19 +1800,19 @@
         <v>168</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="D19" s="4" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F19" s="7" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="20" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1891,19 +1820,19 @@
         <v>169</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>40</v>
+        <v>16</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>41</v>
+        <v>17</v>
       </c>
       <c r="D20" s="4" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E20" s="4" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="21" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1911,19 +1840,19 @@
         <v>170</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>42</v>
+        <v>18</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="F21" s="7" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="22" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1931,19 +1860,19 @@
         <v>171</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>44</v>
+        <v>20</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>45</v>
+        <v>21</v>
       </c>
       <c r="D22" s="4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="F22" s="7" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1951,19 +1880,19 @@
         <v>172</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>46</v>
+        <v>22</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>47</v>
+        <v>23</v>
       </c>
       <c r="D23" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E23" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="24" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1971,19 +1900,19 @@
         <v>173</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>48</v>
+        <v>24</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>49</v>
+        <v>25</v>
       </c>
       <c r="D24" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E24" s="4" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -1991,19 +1920,19 @@
         <v>174</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>50</v>
+        <v>26</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>51</v>
+        <v>27</v>
       </c>
       <c r="D25" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E25" s="4" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="F25" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2011,19 +1940,19 @@
         <v>175</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>28</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>53</v>
+        <v>29</v>
       </c>
       <c r="D26" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E26" s="4" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="27" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2031,19 +1960,19 @@
         <v>176</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>55</v>
+        <v>31</v>
       </c>
       <c r="D27" s="4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="28" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2051,19 +1980,19 @@
         <v>177</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>56</v>
+        <v>32</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>57</v>
+        <v>33</v>
       </c>
       <c r="D28" s="4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E28" s="4" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="29" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2071,19 +2000,19 @@
         <v>178</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>34</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>59</v>
+        <v>35</v>
       </c>
       <c r="D29" s="4" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="E29" s="4" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="30" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2091,19 +2020,19 @@
         <v>179</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>60</v>
+        <v>36</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>61</v>
+        <v>37</v>
       </c>
       <c r="D30" s="4" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E30" s="4" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2111,19 +2040,19 @@
         <v>180</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>63</v>
+        <v>39</v>
       </c>
       <c r="D31" s="4" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="E31" s="4" t="s">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="32" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2131,19 +2060,19 @@
         <v>181</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>64</v>
+        <v>40</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>65</v>
+        <v>41</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E32" s="4" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2151,19 +2080,19 @@
         <v>182</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>66</v>
+        <v>42</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>67</v>
+        <v>43</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="34" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2171,19 +2100,19 @@
         <v>183</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>68</v>
+        <v>44</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>69</v>
+        <v>45</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F34" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="35" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2191,19 +2120,19 @@
         <v>184</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>71</v>
+        <v>47</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="36" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2211,19 +2140,19 @@
         <v>185</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>72</v>
+        <v>48</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>73</v>
+        <v>49</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E36" s="4" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2231,19 +2160,19 @@
         <v>186</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>74</v>
+        <v>50</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>75</v>
+        <v>51</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E37" s="4" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2251,19 +2180,19 @@
         <v>187</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>76</v>
+        <v>52</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="D38" s="4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E38" s="4" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="39" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2271,19 +2200,19 @@
         <v>188</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>79</v>
+        <v>55</v>
       </c>
       <c r="D39" s="4" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="E39" s="4" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2291,19 +2220,19 @@
         <v>189</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>80</v>
+        <v>56</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>81</v>
+        <v>57</v>
       </c>
       <c r="D40" s="4" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E40" s="4" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="41" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2311,19 +2240,19 @@
         <v>190</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>82</v>
+        <v>58</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>83</v>
+        <v>59</v>
       </c>
       <c r="D41" s="4" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="E41" s="4" t="s">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="42" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2331,19 +2260,19 @@
         <v>191</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>84</v>
+        <v>60</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>85</v>
+        <v>61</v>
       </c>
       <c r="D42" s="4" t="s">
-        <v>106</v>
+        <v>88</v>
       </c>
       <c r="E42" s="4" t="s">
-        <v>3</v>
+        <v>89</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="43" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2351,19 +2280,19 @@
         <v>192</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>86</v>
+        <v>62</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>87</v>
+        <v>63</v>
       </c>
       <c r="D43" s="4" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
       <c r="E43" s="4" t="s">
-        <v>3</v>
+        <v>94</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2371,19 +2300,19 @@
         <v>193</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D44" s="4" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="E44" s="4" t="s">
-        <v>3</v>
+        <v>99</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="45" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2391,19 +2320,19 @@
         <v>194</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="C45" s="4" t="s">
-        <v>91</v>
+        <v>67</v>
       </c>
       <c r="D45" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E45" s="4" t="s">
-        <v>3</v>
+        <v>104</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="46" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2411,19 +2340,19 @@
         <v>195</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>92</v>
+        <v>68</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>93</v>
+        <v>69</v>
       </c>
       <c r="D46" s="4" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="E46" s="4" t="s">
-        <v>3</v>
+        <v>109</v>
       </c>
       <c r="F46" s="7" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2431,19 +2360,19 @@
         <v>196</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>94</v>
+        <v>70</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>95</v>
+        <v>71</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>106</v>
+        <v>113</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>3</v>
+        <v>114</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>108</v>
+        <v>115</v>
       </c>
     </row>
     <row r="48" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2451,19 +2380,19 @@
         <v>197</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="C48" s="4" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>106</v>
+        <v>118</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>3</v>
+        <v>119</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>108</v>
+        <v>120</v>
       </c>
     </row>
     <row r="49" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2471,19 +2400,19 @@
         <v>198</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>98</v>
+        <v>74</v>
       </c>
       <c r="C49" s="4" t="s">
-        <v>99</v>
+        <v>75</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>106</v>
+        <v>123</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>3</v>
+        <v>124</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>108</v>
+        <v>125</v>
       </c>
     </row>
     <row r="50" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2491,19 +2420,19 @@
         <v>199</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="D50" s="4" t="s">
-        <v>106</v>
+        <v>128</v>
       </c>
       <c r="E50" s="4" t="s">
-        <v>3</v>
+        <v>129</v>
       </c>
       <c r="F50" s="7" t="s">
-        <v>108</v>
+        <v>130</v>
       </c>
     </row>
     <row r="51" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
@@ -2511,19 +2440,19 @@
         <v>200</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>102</v>
+        <v>78</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
       <c r="D51" s="4" t="s">
-        <v>106</v>
+        <v>133</v>
       </c>
       <c r="E51" s="4" t="s">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="F51" s="7" t="s">
-        <v>108</v>
+        <v>135</v>
       </c>
     </row>
     <row r="52" spans="1:6" ht="13.5" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>